<commit_message>
Livraison CHL v1.2 sans img
</commit_message>
<xml_diff>
--- a/docs/Chiffrage.xlsx
+++ b/docs/Chiffrage.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="28515" windowHeight="12840"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="28515" windowHeight="12840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="CHL" sheetId="4" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
-  <si>
-    <t>Prix</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t xml:space="preserve">Raspberry Pi3
 </t>
@@ -52,12 +49,6 @@
     <t>https://www.amazon.fr/gp/product/B01F1PSFY6/ref=oh_aui_detailpage_o00_s00?ie=UTF8&amp;psc=1</t>
   </si>
   <si>
-    <t>Frais de port</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>https://www.amazon.fr/gp/product/B01H3G1MX2/ref=oh_aui_detailpage_o00_s01?ie=UTF8&amp;psc=1</t>
   </si>
   <si>
@@ -92,6 +83,31 @@
   </si>
   <si>
     <t>TOTAL AVEC 2eme CMD RTC</t>
+  </si>
+  <si>
+    <t>Prix reel</t>
+  </si>
+  <si>
+    <t>Prix CHL</t>
+  </si>
+  <si>
+    <t>Frais de port reel</t>
+  </si>
+  <si>
+    <t>Frais de port chl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Micro PC
+</t>
+  </si>
+  <si>
+    <t>Boîtier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Module horloge </t>
+  </si>
+  <si>
+    <t>Micro SD 16go</t>
   </si>
 </sst>
 </file>
@@ -123,12 +139,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -144,7 +172,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -155,6 +183,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -500,13 +539,13 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>304800</xdr:rowOff>
@@ -977,6 +1016,681 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>23532</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="platop2" descr="iiyama 23&quot; LED - ProLite X2380HS-B1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2333625" y="4514850"/>
+          <a:ext cx="824753" cy="814107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>291041</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>885825</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>733424</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect t="15021" b="14609"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="257175" y="3224741"/>
+          <a:ext cx="628650" cy="442383"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>669163</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect t="17334" b="15556"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="295275" y="4029075"/>
+          <a:ext cx="542925" cy="364363"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>371476</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>323851</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>795117</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>647701</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Image 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect t="11111" b="12444"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="371476" y="4838701"/>
+          <a:ext cx="423641" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="819150" cy="814107"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="platop2" descr="iiyama 23&quot; LED - ProLite X2380HS-B1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2333625" y="5305425"/>
+          <a:ext cx="819150" cy="814107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="824753" cy="819150"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="platop2" descr="iiyama 23&quot; LED - ProLite X2380HS-B1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2333625" y="3724275"/>
+          <a:ext cx="824753" cy="819150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="824753" cy="819150"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="platop2" descr="iiyama 23&quot; LED - ProLite X2380HS-B1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2333625" y="2933700"/>
+          <a:ext cx="824753" cy="819150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="landingImage" descr="Câble micro USB à angle droit - rerii plaqué Doré 30 cm Longueur USB à Micro B mâle à angle droit, câble de charge et synchronisation Micro USB 5 broches câble"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9467850" y="2933700"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>268941</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>966543</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>828673</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Image 10" descr="https://images-eu.ssl-images-amazon.com/images/I/31Sc2atUJIL._SY90_.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="4054" t="12171"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="268941" y="7886700"/>
+          <a:ext cx="697602" cy="638173"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="824753" cy="819150"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="platop2" descr="iiyama 23&quot; LED - ProLite X2380HS-B1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2333625" y="6886575"/>
+          <a:ext cx="824753" cy="819150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="819150" cy="814107"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="platop2" descr="iiyama 23&quot; LED - ProLite X2380HS-B1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2333625" y="7696200"/>
+          <a:ext cx="819150" cy="814107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>280147</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>224118</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>997324</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>702236</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Image 13" descr="https://images-eu.ssl-images-amazon.com/images/I/31nomAG6XsL._SX90_.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="280147" y="7110693"/>
+          <a:ext cx="717177" cy="478118"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="819150" cy="814107"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="platop2" descr="iiyama 23&quot; LED - ProLite X2380HS-B1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2333625" y="6886575"/>
+          <a:ext cx="819150" cy="814107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="824753" cy="819150"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="platop2" descr="iiyama 23&quot; LED - ProLite X2380HS-B1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2333625" y="5305425"/>
+          <a:ext cx="824753" cy="819150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="819150" cy="814107"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="platop2" descr="iiyama 23&quot; LED - ProLite X2380HS-B1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2333625" y="6886575"/>
+          <a:ext cx="819150" cy="814107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>485812</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>997324</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>774670</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Image 18" descr="http://miniimg8.rightinthebox.com/images/384x384/201506/uffgge1434102492199.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="22978" t="15877" r="23100" b="22749"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="485812" y="5495925"/>
+          <a:ext cx="511512" cy="584170"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1267,232 +1981,315 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A7:R20"/>
+  <dimension ref="A7:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="10" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="5">
+        <v>139.96</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:19" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5">
+        <v>29.99</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:19" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
         <v>3</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C10" s="5">
+        <v>39.04</v>
+      </c>
+      <c r="D10" s="5">
         <v>0</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E10" s="7">
+        <v>52.6</v>
+      </c>
+      <c r="F10" s="7">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="G10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="S10">
+        <v>156.16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="5">
+        <v>6.79</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="F11" s="7">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="G11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C8">
-        <v>139.96</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="S11">
+        <v>27.16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="5">
+        <v>5.69</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7">
+        <v>12.95</v>
+      </c>
+      <c r="F12" s="7">
+        <v>7</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S12">
+        <v>22.76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="5">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="D13" s="6">
+        <v>13.72</v>
+      </c>
+      <c r="E13" s="7">
+        <v>48.2</v>
+      </c>
+      <c r="F13" s="8">
+        <v>26</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S13">
+        <v>33.28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="5">
+        <v>2.11</v>
+      </c>
+      <c r="D14" s="6">
+        <v>21.49</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="5">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="D15" s="5">
+        <v>11.96</v>
+      </c>
+      <c r="E15" s="7">
+        <v>13.55</v>
+      </c>
+      <c r="F15" s="7">
+        <v>11.96</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="S15">
+        <v>30.56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="5">
         <v>7</v>
       </c>
-      <c r="C9">
-        <v>29.99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>39.04</v>
-      </c>
-      <c r="D10">
+      <c r="D16" s="5">
         <v>0</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q10">
-        <v>156.16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11">
-        <v>6.79</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="E16" s="7">
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="F16" s="7">
+        <v>8</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="Q11">
-        <v>27.16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12">
-        <v>5.69</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q12">
-        <v>22.76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13">
-        <v>4.8899999999999997</v>
-      </c>
-      <c r="D13" s="4">
-        <v>13.72</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="S16">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="2:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="2:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="2:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="Q13">
-        <v>33.28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14">
-        <v>2.11</v>
-      </c>
-      <c r="D14" s="4">
-        <v>21.49</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15">
-        <v>4.6500000000000004</v>
-      </c>
-      <c r="D15">
-        <v>11.96</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q15">
-        <v>30.56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16">
-        <v>7</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q16">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19">
+      <c r="C19" s="5">
         <f>SUM(C10,C11,C12,C13,C15,C16)*4+SUM(D10:D13,D15,D16)</f>
         <v>297.92</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="5">
         <f>C19/4</f>
         <v>74.48</v>
       </c>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="E19" s="7">
+        <f>SUM(E8:E17)*4</f>
+        <v>611.00000000000011</v>
+      </c>
+      <c r="F19" s="7">
+        <f>SUM(F10:F16)</f>
+        <v>71.960000000000008</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20">
+        <v>21</v>
+      </c>
+      <c r="C20" s="5">
         <f>SUM(C10:C16)*4 + SUM(D10:D16)</f>
         <v>327.84999999999997</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="5">
         <f>C20/4</f>
         <v>81.962499999999991</v>
       </c>
-      <c r="R20">
-        <f>SUM(R10:R16)</f>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="T20">
+        <f>SUM(T10:T16)</f>
         <v>0</v>
       </c>
     </row>
+    <row r="21" spans="2:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="9">
+        <f>SUM(E19:F19)</f>
+        <v>682.96000000000015</v>
+      </c>
+      <c r="F21" s="9"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E21:F21"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E13" r:id="rId1"/>
-    <hyperlink ref="E11" r:id="rId2"/>
-    <hyperlink ref="E16" r:id="rId3"/>
-    <hyperlink ref="E10" r:id="rId4"/>
-    <hyperlink ref="E15" r:id="rId5"/>
-    <hyperlink ref="E12" r:id="rId6"/>
-    <hyperlink ref="E14" r:id="rId7" location=".WG-O7HrW6dM"/>
+    <hyperlink ref="G13" r:id="rId1"/>
+    <hyperlink ref="G11" r:id="rId2"/>
+    <hyperlink ref="G16" r:id="rId3"/>
+    <hyperlink ref="G10" r:id="rId4"/>
+    <hyperlink ref="G15" r:id="rId5"/>
+    <hyperlink ref="G12" r:id="rId6"/>
+    <hyperlink ref="G14" r:id="rId7" location=".WG-O7HrW6dM"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
@@ -1502,13 +2299,196 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A7:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="35" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="5">
+        <v>39.04</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="7">
+        <v>52.6</v>
+      </c>
+      <c r="E8" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="5">
+        <v>6.79</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" s="7">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="5">
+        <v>5.69</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7">
+        <v>12.95</v>
+      </c>
+      <c r="E10" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="5">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="C11" s="6">
+        <v>13.72</v>
+      </c>
+      <c r="D11" s="7">
+        <v>50.2</v>
+      </c>
+      <c r="E11" s="8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="5">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="C12" s="5">
+        <v>11.96</v>
+      </c>
+      <c r="D12" s="7">
+        <v>14.55</v>
+      </c>
+      <c r="E12" s="7">
+        <v>11.96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5">
+        <v>7</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7">
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="E13" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16"/>
+      <c r="B16" s="5">
+        <f>SUM(B8,B9,B10,B11,B12,B13)*4+SUM(C8:C11,C12,C13)</f>
+        <v>297.92</v>
+      </c>
+      <c r="C16" s="5">
+        <f>B16/4</f>
+        <v>74.48</v>
+      </c>
+      <c r="D16" s="7">
+        <f>SUM(D8:D14)*4</f>
+        <v>623.00000000000011</v>
+      </c>
+      <c r="E16" s="7">
+        <f>SUM(E8:E13)</f>
+        <v>76.960000000000008</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17"/>
+      <c r="B17" s="5">
+        <f>SUM(B8:B13)*4 + SUM(C8:C13)</f>
+        <v>297.92</v>
+      </c>
+      <c r="C17" s="5">
+        <f>B17/4</f>
+        <v>74.48</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="D18" s="9">
+        <f>SUM(D16:E16)</f>
+        <v>699.96000000000015</v>
+      </c>
+      <c r="E18" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D18:E18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>